<commit_message>
Primary results of successful optimazation
Run simulation for fewer muscle to save time. Next step is running for all main muscles including recfem_r.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,22 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B045832-F375-4CD3-8F81-5003443BE03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13CFFAA-0ED9-4AF8-941D-AA8292C04FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
+    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$M$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$N$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$1:$J$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$4:$J$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$M$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$N$8</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>bflh_r</t>
   </si>
@@ -73,6 +64,24 @@
   </si>
   <si>
     <t>vasmed_r</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Bounds</t>
+  </si>
+  <si>
+    <t>Optimized 1</t>
+  </si>
+  <si>
+    <t>Optimized 2</t>
+  </si>
+  <si>
+    <t>Optimized 3</t>
   </si>
 </sst>
 </file>
@@ -218,7 +227,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -256,7 +265,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$J$4</c:f>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1074,15 +1083,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>552449</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1408,150 +1417,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0.30803025314489302</v>
-      </c>
-      <c r="B2">
-        <v>4.7219446633879697E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.41609463602934499</v>
-      </c>
-      <c r="D2">
-        <v>0.43916405262658997</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>0.48245563417203602</v>
+        <v>0.49444199999999999</v>
       </c>
       <c r="F2">
-        <v>0.32341642618330702</v>
+        <v>0.43676900000000002</v>
       </c>
       <c r="G2">
-        <v>0.229396111076588</v>
+        <v>0.41691299999999998</v>
       </c>
       <c r="H2">
-        <v>0.31963109767354098</v>
+        <v>0.47110800000000003</v>
       </c>
       <c r="I2">
-        <v>0.19086280211019499</v>
+        <v>0.27967799999999998</v>
       </c>
       <c r="J2">
-        <v>0.181274563686359</v>
+        <v>0.29267900000000002</v>
+      </c>
+      <c r="K2">
+        <v>0.268264</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>0.31790000000000002</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.104</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.432</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.45700000000000002</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.124</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.33</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.245</v>
-      </c>
-      <c r="H3">
-        <v>0.2</v>
       </c>
       <c r="I3">
         <v>0.2</v>
       </c>
       <c r="J3">
+        <v>0.2</v>
+      </c>
+      <c r="K3">
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>(A2-A3)/A3*100</f>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.30803025314489302</v>
+      </c>
+      <c r="C4">
+        <v>4.7219446633879697E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.41609463602934499</v>
+      </c>
+      <c r="E4">
+        <v>0.43916405262658997</v>
+      </c>
+      <c r="F4">
+        <v>0.48245563417203602</v>
+      </c>
+      <c r="G4">
+        <v>0.32341642618330702</v>
+      </c>
+      <c r="H4">
+        <v>0.229396111076588</v>
+      </c>
+      <c r="I4">
+        <v>0.31963109767354098</v>
+      </c>
+      <c r="J4">
+        <v>0.19086280211019499</v>
+      </c>
+      <c r="K4">
+        <v>0.181274563686359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <f>(B4-B3)/B3*100</f>
         <v>-3.1046702910056614</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:J4" si="0">(B2-B3)/B3*100</f>
+      <c r="C5">
+        <f>(C4-C3)/C3*100</f>
         <v>-54.596685928961833</v>
       </c>
-      <c r="C4">
+      <c r="D5">
+        <f>(D4-D3)/D3*100</f>
+        <v>-3.6817972154294001</v>
+      </c>
+      <c r="E5">
+        <f>(E4-E3)/E3*100</f>
+        <v>-3.9028331232844735</v>
+      </c>
+      <c r="F5">
+        <f>(F4-F3)/F3*100</f>
+        <v>289.0771243322871</v>
+      </c>
+      <c r="G5">
+        <f>(G4-G3)/G3*100</f>
+        <v>-1.9950223686948483</v>
+      </c>
+      <c r="H5">
+        <f>(H4-H3)/H3*100</f>
+        <v>-6.3689342544538761</v>
+      </c>
+      <c r="I5">
+        <f>(I4-I3)/I3*100</f>
+        <v>59.815548836770482</v>
+      </c>
+      <c r="J5">
+        <f>(J4-J3)/J3*100</f>
+        <v>-4.5685989449025106</v>
+      </c>
+      <c r="K5">
+        <f>(K4-K3)/K3*100</f>
+        <v>-8.4471900573944509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>0.33814333513871703</v>
+      </c>
+      <c r="H6">
+        <v>0.24548721408889099</v>
+      </c>
+      <c r="I6">
+        <v>0.198664661813162</v>
+      </c>
+      <c r="J6">
+        <v>0.2203206165746</v>
+      </c>
+      <c r="K6">
+        <v>0.19694217863267499</v>
+      </c>
+      <c r="M6">
+        <v>0.198664661813162</v>
+      </c>
+      <c r="N6">
+        <v>0.2203206165746</v>
+      </c>
+      <c r="O6">
+        <v>0.19694217863267499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="e">
+        <f>(B5-B6)/B6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" t="e">
+        <f t="shared" ref="C7:F7" si="0">(C5-C6)/C6*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D7" t="e">
         <f t="shared" si="0"/>
-        <v>-3.6817972154294001</v>
-      </c>
-      <c r="D4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" t="e">
         <f t="shared" si="0"/>
-        <v>-3.9028331232844735</v>
-      </c>
-      <c r="E4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" t="e">
         <f t="shared" si="0"/>
-        <v>289.0771243322871</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>-1.9950223686948483</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>-6.3689342544538761</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>59.815548836770482</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>-4.5685989449025106</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>-8.4471900573944509</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7">
+        <f>(G4-G6)/G6*100</f>
+        <v>-4.3552267411595054</v>
+      </c>
+      <c r="H7">
+        <f>(H4-H6)/H6*100</f>
+        <v>-6.5547621581938662</v>
+      </c>
+      <c r="I7">
+        <f>(I4-I6)/I6*100</f>
+        <v>60.889760039027067</v>
+      </c>
+      <c r="J7">
+        <f>(J4-J6)/J6*100</f>
+        <v>-13.370430294901917</v>
+      </c>
+      <c r="K7">
+        <f>(K4-K6)/K6*100</f>
+        <v>-7.9554390304264437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>0.45688976686243499</v>
+      </c>
+      <c r="F8">
+        <v>0.279706945394611</v>
+      </c>
+      <c r="G8">
+        <v>0.33815164689752603</v>
+      </c>
+      <c r="H8">
+        <v>0.24555804731407799</v>
+      </c>
+      <c r="I8">
+        <v>0.19619101991282401</v>
+      </c>
+      <c r="J8">
+        <v>0.21105392695196401</v>
+      </c>
+      <c r="K8">
+        <v>0.19329936476910001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>(B8-B$3)/B$3*100</f>
+        <v>-100</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:K9" si="1">(C8-C$3)/C$3*100</f>
+        <v>-100</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-2.4121036666308545E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>125.57011725371854</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2.4701960295533363</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.22777441390938441</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>-1.904490043588003</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>5.5269634759819999</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>-2.3740581974242434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MOCO did not converge with all muscles
Modified the model to have following muscles:
bflh_r, bfsh_r, gaslat_r, gasmed_r, sart_r, semimem_r, semiten_r,  vasint_r, vaslat_r, vasmed_r
run simulation to  find the tendon slack length. it did not converge.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13CFFAA-0ED9-4AF8-941D-AA8292C04FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4112A950-35F9-4D4C-9EDA-D59F83BCE6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>bflh_r</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Optimized 3</t>
+  </si>
+  <si>
+    <t>recfem_r</t>
+  </si>
+  <si>
+    <t>tfl_r</t>
+  </si>
+  <si>
+    <t>Wrong</t>
   </si>
 </sst>
 </file>
@@ -1083,16 +1092,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1417,15 +1426,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1561,43 +1571,43 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <f>(B4-B3)/B3*100</f>
+        <f t="shared" ref="B5:K5" si="0">(B4-B3)/B3*100</f>
         <v>-3.1046702910056614</v>
       </c>
       <c r="C5">
-        <f>(C4-C3)/C3*100</f>
+        <f t="shared" si="0"/>
         <v>-54.596685928961833</v>
       </c>
       <c r="D5">
-        <f>(D4-D3)/D3*100</f>
+        <f t="shared" si="0"/>
         <v>-3.6817972154294001</v>
       </c>
       <c r="E5">
-        <f>(E4-E3)/E3*100</f>
+        <f t="shared" si="0"/>
         <v>-3.9028331232844735</v>
       </c>
       <c r="F5">
-        <f>(F4-F3)/F3*100</f>
+        <f t="shared" si="0"/>
         <v>289.0771243322871</v>
       </c>
       <c r="G5">
-        <f>(G4-G3)/G3*100</f>
+        <f t="shared" si="0"/>
         <v>-1.9950223686948483</v>
       </c>
       <c r="H5">
-        <f>(H4-H3)/H3*100</f>
+        <f t="shared" si="0"/>
         <v>-6.3689342544538761</v>
       </c>
       <c r="I5">
-        <f>(I4-I3)/I3*100</f>
+        <f t="shared" si="0"/>
         <v>59.815548836770482</v>
       </c>
       <c r="J5">
-        <f>(J4-J3)/J3*100</f>
+        <f t="shared" si="0"/>
         <v>-4.5685989449025106</v>
       </c>
       <c r="K5">
-        <f>(K4-K3)/K3*100</f>
+        <f t="shared" si="0"/>
         <v>-8.4471900573944509</v>
       </c>
     </row>
@@ -1639,19 +1649,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C7" t="e">
-        <f t="shared" ref="C7:F7" si="0">(C5-C6)/C6*100</f>
+        <f t="shared" ref="C7:F7" si="1">(C5-C6)/C6*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D7" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E7" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F7" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G7">
@@ -1710,44 +1720,234 @@
         <v>-100</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:K9" si="1">(C8-C$3)/C$3*100</f>
+        <f t="shared" ref="C9:K9" si="2">(C8-C$3)/C$3*100</f>
         <v>-100</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-100</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4121036666308545E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>125.57011725371854</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4701960295533363</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22777441390938441</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.904490043588003</v>
       </c>
       <c r="J9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5269634759819999</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.3740581974242434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.31640318320961602</v>
+      </c>
+      <c r="C10">
+        <v>3.6175111501355502E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.42307125921227901</v>
+      </c>
+      <c r="E10">
+        <v>0.45534746482990202</v>
+      </c>
+      <c r="F10">
+        <v>0.34404369494548898</v>
+      </c>
+      <c r="G10">
+        <v>0.33697344893764403</v>
+      </c>
+      <c r="H10">
+        <v>0.24194566064363099</v>
+      </c>
+      <c r="I10">
+        <v>0.25152103002840998</v>
+      </c>
+      <c r="J10">
+        <v>0.27967796671973</v>
+      </c>
+      <c r="K10">
+        <v>0.181427770834516</v>
+      </c>
+      <c r="L10">
+        <v>0.169847988826857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.31790000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.104</v>
+      </c>
+      <c r="D12">
+        <v>0.432</v>
+      </c>
+      <c r="E12">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="F12">
+        <v>0.42</v>
+      </c>
+      <c r="G12">
+        <v>0.41691299999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.47110800000000003</v>
+      </c>
+      <c r="I12">
+        <v>0.25</v>
+      </c>
+      <c r="J12">
+        <v>0.27967799999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.29267900000000002</v>
+      </c>
+      <c r="L12">
+        <v>0.268264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.31640318320961602</v>
+      </c>
+      <c r="C13">
+        <v>3.6175111501355502E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.42307125921227901</v>
+      </c>
+      <c r="E13">
+        <v>0.45534746482990202</v>
+      </c>
+      <c r="F13">
+        <v>0.34404369494548898</v>
+      </c>
+      <c r="G13">
+        <v>0.33697344893764403</v>
+      </c>
+      <c r="H13">
+        <v>0.24194566064363099</v>
+      </c>
+      <c r="I13">
+        <v>0.25152103002840998</v>
+      </c>
+      <c r="J13">
+        <v>0.27967796671973</v>
+      </c>
+      <c r="K13">
+        <v>0.181427770834516</v>
+      </c>
+      <c r="L13">
+        <v>0.169847988826857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ref="B14" si="3">(B13-B12)/B12*100</f>
+        <v>-0.47084516841270596</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14" si="4">(C13-C12)/C12*100</f>
+        <v>-65.216238941004306</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="5">(D13-D12)/D12*100</f>
+        <v>-2.0668381453057849</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="6">(E13-E12)/E12*100</f>
+        <v>-0.36160507004332643</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14" si="7">(F13-F12)/F12*100</f>
+        <v>-18.084834536788335</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="8">(G13-G12)/G12*100</f>
+        <v>-19.174156493646386</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14" si="9">(H13-H12)/H12*100</f>
+        <v>-48.643270620827714</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14" si="10">(I13-I12)/I12*100</f>
+        <v>0.60841201136399015</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14" si="11">(J13-J12)/J12*100</f>
+        <v>-1.1899495128069271E-5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14" si="12">(K13-K12)/K12*100</f>
+        <v>-38.011346617107485</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14" si="13">(L13-L12)/L12*100</f>
+        <v>-36.686253531276279</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Result for all muscle, full range of motion
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47934D7-3862-4A5B-B958-F9E366BDB8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5812F45-9D5B-4E0F-80B3-8FFC4F1F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>bflh_r</t>
   </si>
@@ -93,7 +93,10 @@
     <t>Wrong</t>
   </si>
   <si>
-    <t>First try0to5s</t>
+    <t>0-90deg</t>
+  </si>
+  <si>
+    <t>0-22.5deg</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,492 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0-22.5deg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$L$11</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tfl_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.7017879870076491E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.262963230640402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.96461782219143222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.0058639844623714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11.72965497233595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7898153400174522E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12257866653788974</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.3617938863996759E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12430797850449669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3982869364470933</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3159914411376019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DA8F-470A-B28E-0458A094B5C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0-90deg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.1770819634783211E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.078782552175003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.52451797603911587</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.89243229781597688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.5999371755035625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0417409653061335E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4134409118985118E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.1949290747992336E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.1682980073855308E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18384511149015528</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.8194351084163108E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DA8F-470A-B28E-0458A094B5C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="420355295"/>
+        <c:axId val="420352799"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="420355295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420352799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420352799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420355295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1091,19 +1579,513 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1124,6 +2106,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21443294-1E6B-4ECB-ADA7-28100EBA6B89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1429,15 +2447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="7" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1948,53 +2966,53 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <f>(B14-B13)/B13*100</f>
+        <f t="shared" ref="B15:L15" si="3">(B14-B13)/B13*100</f>
         <v>-0.47084516841270596</v>
       </c>
       <c r="C15">
-        <f>(C14-C13)/C13*100</f>
+        <f t="shared" si="3"/>
         <v>-65.216238941004306</v>
       </c>
       <c r="D15">
-        <f>(D14-D13)/D13*100</f>
+        <f t="shared" si="3"/>
         <v>-2.0668381453057849</v>
       </c>
       <c r="E15">
-        <f>(E14-E13)/E13*100</f>
+        <f t="shared" si="3"/>
         <v>-0.36160507004332643</v>
       </c>
       <c r="F15">
-        <f>(F14-F13)/F13*100</f>
+        <f t="shared" si="3"/>
         <v>-18.084834536788335</v>
       </c>
       <c r="G15">
-        <f>(G14-G13)/G13*100</f>
+        <f t="shared" si="3"/>
         <v>-0.3332005508299275</v>
       </c>
       <c r="H15">
-        <f>(H14-H13)/H13*100</f>
+        <f t="shared" si="3"/>
         <v>-1.4076362495391272</v>
       </c>
       <c r="I15">
-        <f>(I14-I13)/I13*100</f>
+        <f t="shared" si="3"/>
         <v>0.60841201136399015</v>
       </c>
       <c r="J15">
-        <f>(J14-J13)/J13*100</f>
+        <f t="shared" si="3"/>
         <v>39.5598636325998</v>
       </c>
       <c r="K15">
-        <f>(K14-K13)/K13*100</f>
+        <f t="shared" si="3"/>
         <v>-16.890622613597799</v>
       </c>
       <c r="L15">
-        <f>(L14-L13)/L13*100</f>
+        <f t="shared" si="3"/>
         <v>-14.391134663882553</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>0.31808125984010699</v>
@@ -2030,50 +3048,134 @@
         <v>0.201010927019217</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>(B16-B$13)/B$13*100</f>
         <v>5.7017879870076491E-2</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:L17" si="3">(C16-C$13)/C$13*100</f>
+        <f t="shared" ref="C17:L17" si="4">(C16-C$13)/C$13*100</f>
         <v>32.262963230640402</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.96461782219143222</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.0058639844623714</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-11.72965497233595</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7898153400174522E-2</v>
       </c>
       <c r="H17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12257866653788974</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1.3617938863996759E-2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12430797850449669</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3982869364470933</v>
       </c>
       <c r="L17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3159914411376019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>0.31800099943561899</v>
+      </c>
+      <c r="C18">
+        <v>0.121761933854262</v>
+      </c>
+      <c r="D18">
+        <v>0.42973408234351101</v>
+      </c>
+      <c r="E18">
+        <v>0.452921584398981</v>
+      </c>
+      <c r="F18">
+        <v>0.40068026386288502</v>
+      </c>
+      <c r="G18">
+        <v>0.33816903126203701</v>
+      </c>
+      <c r="H18">
+        <v>0.245483765839978</v>
+      </c>
+      <c r="I18">
+        <v>0.249997012677313</v>
+      </c>
+      <c r="J18">
+        <v>0.20021626730793199</v>
+      </c>
+      <c r="K18">
+        <v>0.218701333878383</v>
+      </c>
+      <c r="L18">
+        <v>0.19832422240744901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>(B18-B$13)/B$13*100</f>
+        <v>3.1770819634783211E-2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:L19" si="5">(C18-C$13)/C$13*100</f>
+        <v>17.078782552175003</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="5"/>
+        <v>-0.52451797603911587</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="5"/>
+        <v>-0.89243229781597688</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>-4.5999371755035625</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>2.0417409653061335E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="5"/>
+        <v>3.4134409118985118E-2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>-1.1949290747992336E-3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>-9.1682980073855308E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>0.18384511149015528</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>-3.8194351084163108E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two parameter optimization result for all muscles
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5812F45-9D5B-4E0F-80B3-8FFC4F1F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1086CC61-CB1A-4207-B9D3-98C64E085506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>bflh_r</t>
   </si>
@@ -97,6 +97,81 @@
   </si>
   <si>
     <t>0-22.5deg</t>
+  </si>
+  <si>
+    <t>tendon_slack_bflh_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcebflh_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_bfsh_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcebfsh_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_gaslat_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcegaslat_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_gasmed_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcegasmed_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_recfem_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcerecfem_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_semimem_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcesemimem_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_semiten_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcesemiten_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_tfl_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcetfl_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_vasint_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcevasint_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_vaslat_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcevaslat_r</t>
+  </si>
+  <si>
+    <t>tendon_slack_vasmed_r</t>
+  </si>
+  <si>
+    <t>passive_fiber_strain_at_one_norm_forcevasmed_r</t>
+  </si>
+  <si>
+    <t>Passive parameter</t>
+  </si>
+  <si>
+    <t>Tendon Slack length</t>
+  </si>
+  <si>
+    <t>Second try</t>
   </si>
 </sst>
 </file>
@@ -132,8 +207,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,7 +323,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:f>Sheet1!$C$1:$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -280,7 +361,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$K$5</c:f>
+              <c:f>Sheet1!$C$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -638,7 +719,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$11:$L$11</c:f>
+              <c:f>Sheet1!$C$11:$M$11</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -679,7 +760,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$L$17</c:f>
+              <c:f>Sheet1!$C$17:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -752,7 +833,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$L$19</c:f>
+              <c:f>Sheet1!$C$19:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2077,13 +2158,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>314326</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2113,16 +2194,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>14285</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2447,234 +2528,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="7" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="8" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.49444199999999999</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.43676900000000002</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.41691299999999998</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.47110800000000003</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.27967799999999998</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.29267900000000002</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.268264</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.31790000000000002</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.104</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.432</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.45700000000000002</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.124</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.33</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.245</v>
-      </c>
-      <c r="I3">
-        <v>0.2</v>
       </c>
       <c r="J3">
         <v>0.2</v>
       </c>
       <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3">
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.30803025314489302</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>4.7219446633879697E-2</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.41609463602934499</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.43916405262658997</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.48245563417203602</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.32341642618330702</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.229396111076588</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.31963109767354098</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.19086280211019499</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.181274563686359</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <f t="shared" ref="B5:K5" si="0">(B4-B3)/B3*100</f>
+      <c r="C5">
+        <f t="shared" ref="C5:L5" si="0">(C4-C3)/C3*100</f>
         <v>-3.1046702910056614</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>-54.596685928961833</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>-3.6817972154294001</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>-3.9028331232844735</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>289.0771243322871</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>-1.9950223686948483</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>-6.3689342544538761</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>59.815548836770482</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>-4.5685989449025106</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="0"/>
         <v>-8.4471900573944509</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.33814333513871703</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.24548721408889099</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.198664661813162</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.2203206165746</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.19694217863267499</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.198664661813162</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.2203206165746</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.19694217863267499</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="e">
-        <f>(B5-B6)/B6*100</f>
+      <c r="C7" t="e">
+        <f>(C5-C6)/C6*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C7" t="e">
-        <f t="shared" ref="C7:F7" si="1">(C5-C6)/C6*100</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="D7" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D7:G7" si="1">(D5-D6)/D6*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E7" t="e">
@@ -2685,500 +2762,822 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7">
-        <f>(G4-G6)/G6*100</f>
-        <v>-4.3552267411595054</v>
+      <c r="G7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="H7">
         <f>(H4-H6)/H6*100</f>
-        <v>-6.5547621581938662</v>
+        <v>-4.3552267411595054</v>
       </c>
       <c r="I7">
         <f>(I4-I6)/I6*100</f>
-        <v>60.889760039027067</v>
+        <v>-6.5547621581938662</v>
       </c>
       <c r="J7">
         <f>(J4-J6)/J6*100</f>
-        <v>-13.370430294901917</v>
+        <v>60.889760039027067</v>
       </c>
       <c r="K7">
         <f>(K4-K6)/K6*100</f>
+        <v>-13.370430294901917</v>
+      </c>
+      <c r="L7">
+        <f>(L4-L6)/L6*100</f>
         <v>-7.9554390304264437</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.45688976686243499</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.279706945394611</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.33815164689752603</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.24555804731407799</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.19619101991282401</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.21105392695196401</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.19329936476910001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <f>(B8-B$3)/B$3*100</f>
+      <c r="C9">
+        <f>(C8-C$3)/C$3*100</f>
         <v>-100</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:K9" si="2">(C8-C$3)/C$3*100</f>
+      <c r="D9">
+        <f t="shared" ref="D9:L9" si="2">(D8-D$3)/D$3*100</f>
         <v>-100</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="2"/>
         <v>-2.4121036666308545E-2</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="2"/>
         <v>125.57011725371854</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="2"/>
         <v>2.4701960295533363</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="2"/>
         <v>0.22777441390938441</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>-1.904490043588003</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>5.5269634759819999</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="2"/>
         <v>-2.3740581974242434</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>0.31640318320961602</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>3.6175111501355502E-2</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.42307125921227901</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.45534746482990202</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.34404369494548898</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.33697344893764403</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.24194566064363099</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.25152103002840998</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.27967796671973</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.181427770834516</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>0.169847988826857</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>5</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>7</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>8</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.44521300000000003</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.180864</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.48099999999999998</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.49440000000000001</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.42159999999999997</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.41689999999999999</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.47099999999999997</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.43730000000000002</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.27900000000000003</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>0.29267900000000002</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.31790000000000002</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.104</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.432</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.45700000000000002</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0.42</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.33810000000000001</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.24540000000000001</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.25</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.20039999999999999</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.21829999999999999</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.19839999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.31640318320961602</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>3.6175111501355502E-2</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.42307125921227901</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.45534746482990202</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.34404369494548898</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.33697344893764403</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.24194566064363099</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.25152103002840998</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.27967796671973</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.181427770834516</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.169847988826857</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <f t="shared" ref="B15:L15" si="3">(B14-B13)/B13*100</f>
+      <c r="C15">
+        <f t="shared" ref="C15:M15" si="3">(C14-C13)/C13*100</f>
         <v>-0.47084516841270596</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <f t="shared" si="3"/>
         <v>-65.216238941004306</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="3"/>
         <v>-2.0668381453057849</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f t="shared" si="3"/>
         <v>-0.36160507004332643</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <f t="shared" si="3"/>
         <v>-18.084834536788335</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="3"/>
         <v>-0.3332005508299275</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="3"/>
         <v>-1.4076362495391272</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="3"/>
         <v>0.60841201136399015</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="3"/>
         <v>39.5598636325998</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f t="shared" si="3"/>
         <v>-16.890622613597799</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="3"/>
         <v>-14.391134663882553</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.31808125984010699</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.13755348175986601</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0.42783285100813301</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>0.44783320159100698</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.370735449116189</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.338228133656646</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.24570080804768399</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.24996595515284001</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.20064911318892301</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.221352460382264</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>0.201010927019217</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>(B16-B$13)/B$13*100</f>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>(C16-C$13)/C$13*100</f>
         <v>5.7017879870076491E-2</v>
       </c>
-      <c r="C17">
-        <f t="shared" ref="C17:L17" si="4">(C16-C$13)/C$13*100</f>
+      <c r="D17">
+        <f t="shared" ref="D17:M17" si="4">(D16-D$13)/D$13*100</f>
         <v>32.262963230640402</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="4"/>
         <v>-0.96461782219143222</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f t="shared" si="4"/>
         <v>-2.0058639844623714</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f t="shared" si="4"/>
         <v>-11.72965497233595</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="4"/>
         <v>3.7898153400174522E-2</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="4"/>
         <v>0.12257866653788974</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="4"/>
         <v>-1.3617938863996759E-2</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="4"/>
         <v>0.12430797850449669</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <f t="shared" si="4"/>
         <v>1.3982869364470933</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="4"/>
         <v>1.3159914411376019</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.31800099943561899</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.121761933854262</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.42973408234351101</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>0.452921584398981</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>0.40068026386288502</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.33816903126203701</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.245483765839978</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>0.249997012677313</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.20021626730793199</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>0.218701333878383</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>0.19832422240744901</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f>(B18-B$13)/B$13*100</f>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19">
+        <f>(C18-C$13)/C$13*100</f>
         <v>3.1770819634783211E-2</v>
       </c>
-      <c r="C19">
-        <f t="shared" ref="C19:L19" si="5">(C18-C$13)/C$13*100</f>
+      <c r="D19">
+        <f t="shared" ref="D19:M19" si="5">(D18-D$13)/D$13*100</f>
         <v>17.078782552175003</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <f t="shared" si="5"/>
         <v>-0.52451797603911587</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f t="shared" si="5"/>
         <v>-0.89243229781597688</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <f t="shared" si="5"/>
         <v>-4.5999371755035625</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="5"/>
         <v>2.0417409653061335E-2</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="5"/>
         <v>3.4134409118985118E-2</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="5"/>
         <v>-1.1949290747992336E-3</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="5"/>
         <v>-9.1682980073855308E-2</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <f t="shared" si="5"/>
         <v>0.18384511149015528</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f t="shared" si="5"/>
         <v>-3.8194351084163108E-2</v>
       </c>
     </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20">
+        <v>0.317928889160771</v>
+      </c>
+      <c r="D20">
+        <v>0.17060450569378599</v>
+      </c>
+      <c r="E20">
+        <v>0.42704459805116801</v>
+      </c>
+      <c r="F20">
+        <v>0.44820414428845101</v>
+      </c>
+      <c r="G20">
+        <v>0.39747425206256698</v>
+      </c>
+      <c r="H20">
+        <v>0.33835910801271601</v>
+      </c>
+      <c r="I20">
+        <v>0.245525369483062</v>
+      </c>
+      <c r="J20">
+        <v>0.24984576653162099</v>
+      </c>
+      <c r="K20">
+        <v>0.20014376388077901</v>
+      </c>
+      <c r="L20">
+        <v>0.22289587902927099</v>
+      </c>
+      <c r="M20">
+        <v>0.200618994686414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21">
+        <f>(C20-C$13)/C$13*100</f>
+        <v>9.0874994561132502E-3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:M21" si="6">(D20-D$13)/D$13*100</f>
+        <v>64.042793936332686</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>-1.147083784451848</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>-1.9246949040588632</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>-5.3632733184364296</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>7.6636501838510146E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>5.1087808908717752E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>-6.1693387351602347E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>-0.12786233494061239</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="6"/>
+        <v>2.1053041819839668</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="6"/>
+        <v>1.1184449024264167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
+        <v>0.70079674064287201</v>
+      </c>
+      <c r="D22">
+        <v>0.70802054936171999</v>
+      </c>
+      <c r="E22">
+        <v>0.69693452886853102</v>
+      </c>
+      <c r="F22">
+        <v>0.69395337088414799</v>
+      </c>
+      <c r="G22">
+        <v>0.79999999359030105</v>
+      </c>
+      <c r="H22">
+        <v>0.69726547708197295</v>
+      </c>
+      <c r="I22">
+        <v>0.69993572020314598</v>
+      </c>
+      <c r="J22">
+        <v>0.70133491580469098</v>
+      </c>
+      <c r="K22">
+        <v>0.69963467516214195</v>
+      </c>
+      <c r="L22">
+        <v>0.56783493142832098</v>
+      </c>
+      <c r="M22">
+        <v>0.63613288686708103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23">
+        <f>(C22-0.7)/0.7*100</f>
+        <v>0.11382009183886449</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:M23" si="7">(D22-0.7)/0.7*100</f>
+        <v>1.1457927659600045</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>-0.43792444735270475</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>-0.8638041594074235</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>14.285713370043016</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>-0.39064613114671498</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>-9.182828121996018E-3</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="7"/>
+        <v>0.19070225781300404</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>-5.2189262551143631E-2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>-18.880724081668426</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>-9.1238733047027054</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" t="s">
+        <v>29</v>
+      </c>
+      <c r="K44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L44" t="s">
+        <v>31</v>
+      </c>
+      <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O44" t="s">
+        <v>34</v>
+      </c>
+      <c r="P44" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>36</v>
+      </c>
+      <c r="R44" t="s">
+        <v>37</v>
+      </c>
+      <c r="S44" t="s">
+        <v>38</v>
+      </c>
+      <c r="T44" t="s">
+        <v>39</v>
+      </c>
+      <c r="U44" t="s">
+        <v>40</v>
+      </c>
+      <c r="V44" t="s">
+        <v>41</v>
+      </c>
+      <c r="W44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.317928889160771</v>
+      </c>
+      <c r="C45">
+        <v>0.70079674064287201</v>
+      </c>
+      <c r="D45">
+        <v>0.17060450569378599</v>
+      </c>
+      <c r="E45">
+        <v>0.70802054936171999</v>
+      </c>
+      <c r="F45">
+        <v>0.42704459805116801</v>
+      </c>
+      <c r="G45">
+        <v>0.69693452886853102</v>
+      </c>
+      <c r="H45">
+        <v>0.44820414428845101</v>
+      </c>
+      <c r="I45">
+        <v>0.69395337088414799</v>
+      </c>
+      <c r="J45">
+        <v>0.39747425206256698</v>
+      </c>
+      <c r="K45">
+        <v>0.79999999359030105</v>
+      </c>
+      <c r="L45">
+        <v>0.33835910801271601</v>
+      </c>
+      <c r="M45">
+        <v>0.69726547708197295</v>
+      </c>
+      <c r="N45">
+        <v>0.245525369483062</v>
+      </c>
+      <c r="O45">
+        <v>0.69993572020314598</v>
+      </c>
+      <c r="P45">
+        <v>0.24984576653162099</v>
+      </c>
+      <c r="Q45">
+        <v>0.70133491580469098</v>
+      </c>
+      <c r="R45">
+        <v>0.20014376388077901</v>
+      </c>
+      <c r="S45">
+        <v>0.69963467516214195</v>
+      </c>
+      <c r="T45">
+        <v>0.22289587902927099</v>
+      </c>
+      <c r="U45">
+        <v>0.56783493142832098</v>
+      </c>
+      <c r="V45">
+        <v>0.200618994686414</v>
+      </c>
+      <c r="W45">
+        <v>0.63613288686708103</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A20:A23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Parameter optimization on 45deg Hip, a main script added to run all functions together
During simulation I figured out tlf creates hug amount of passive force in hip 45 and I deiced to remove this muscle from simulation. Results shows weaker estimation. It makes sense because in Hip 45 muscles are less involved to create passive force.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1086CC61-CB1A-4207-B9D3-98C64E085506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7489C32-3570-46C9-8064-E8344D6D38BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
+    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>bflh_r</t>
   </si>
@@ -210,10 +210,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,6 +646,66 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Tendon Slack lenght_Hip90</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="15"/>
@@ -876,6 +936,917 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-DA8F-470A-B28E-0458A094B5C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="420355295"/>
+        <c:axId val="420352799"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="420355295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420352799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420352799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420355295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tendon Slack lenght_Hip45</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$11:$M$11</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tfl_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$25:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-13.480881554001256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73.907741591675006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0625237167818867E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1216648611369824E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0966122676169041</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11.230727038449572</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-19.68198090378117</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.56590636064121447</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.2518232328016416</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.88758949080745098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACC6-4B96-BD35-7AC2FA5A0E77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="984742879"/>
+        <c:axId val="984746623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="984742879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984746623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="984746623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+          <c:min val="-30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984742879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Tendon Slack lenght_Hip90</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tendon Slack length</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$11:$M$11</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tfl_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$21:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.0874994561132502E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.042793936332686</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.147083784451848</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.9246949040588632</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.3632733184364296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6636501838510146E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1087808908717752E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-6.1693387351602347E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.12786233494061239</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1053041819839668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1184449024264167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1598-4454-B590-1F1EB00232A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Passive parameter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.11382009183886449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1457927659600045</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.43792444735270475</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.8638041594074235</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.285713370043016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.39064613114671498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9.182828121996018E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19070225781300404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.2189262551143631E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-18.880724081668426</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.1238733047027054</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1598-4454-B590-1F1EB00232A0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1157,6 +2128,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1661,6 +2712,1003 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2195,15 +4243,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14286</xdr:rowOff>
+      <xdr:colOff>318247</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>70315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>291354</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>99593</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2223,6 +4271,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>78440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>463364</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>42583</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A79D7F4D-A9AD-4945-B823-08C85F4F3776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>246530</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>185363</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2912B6C-2027-45F2-B9D9-3E265CCFAF58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2530,8 +4654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,7 +5338,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="1"/>
       <c r="C19">
         <f>(C18-C$13)/C$13*100</f>
         <v>3.1770819634783211E-2</v>
@@ -3261,10 +5385,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C20">
@@ -3302,8 +5426,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21">
         <f>(C20-C$13)/C$13*100</f>
         <v>9.0874994561132502E-3</v>
@@ -3350,8 +5474,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C22">
@@ -3389,8 +5513,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23">
         <f>(C22-0.7)/0.7*100</f>
         <v>0.11382009183886449</v>
@@ -3434,6 +5558,88 @@
       <c r="M23">
         <f t="shared" si="7"/>
         <v>-9.1238733047027054</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>0.27504427753983002</v>
+      </c>
+      <c r="D24">
+        <v>0.180864051255342</v>
+      </c>
+      <c r="E24">
+        <v>0.43239150102456497</v>
+      </c>
+      <c r="F24">
+        <v>0.45718836008415398</v>
+      </c>
+      <c r="G24">
+        <v>0.44980577152399098</v>
+      </c>
+      <c r="H24">
+        <v>0.300128911883002</v>
+      </c>
+      <c r="I24">
+        <v>0.19710041886212101</v>
+      </c>
+      <c r="K24">
+        <v>0.199265923653275</v>
+      </c>
+      <c r="L24">
+        <v>0.21556726988279401</v>
+      </c>
+      <c r="M24">
+        <v>0.19663902245023801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25">
+        <f>(C24-C$13)/C$13*100</f>
+        <v>-13.480881554001256</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:M25" si="8">(D24-D$13)/D$13*100</f>
+        <v>73.907741591675006</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="8"/>
+        <v>9.0625237167818867E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="8"/>
+        <v>4.1216648611369824E-2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="8"/>
+        <v>7.0966122676169041</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="8"/>
+        <v>-11.230727038449572</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="8"/>
+        <v>-19.68198090378117</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="8"/>
+        <v>-100</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="8"/>
+        <v>-0.56590636064121447</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="8"/>
+        <v>-1.2518232328016416</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>-0.88758949080745098</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -3573,10 +5779,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Parameter Opt for Hip=0
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7489C32-3570-46C9-8064-E8344D6D38BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4881C686-4808-463C-8CA3-753A4EEED6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>bflh_r</t>
   </si>
@@ -99,72 +99,6 @@
     <t>0-22.5deg</t>
   </si>
   <si>
-    <t>tendon_slack_bflh_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcebflh_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_bfsh_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcebfsh_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_gaslat_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcegaslat_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_gasmed_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcegasmed_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_recfem_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcerecfem_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_semimem_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcesemimem_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_semiten_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcesemiten_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_tfl_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcetfl_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_vasint_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcevasint_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_vaslat_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcevaslat_r</t>
-  </si>
-  <si>
-    <t>tendon_slack_vasmed_r</t>
-  </si>
-  <si>
-    <t>passive_fiber_strain_at_one_norm_forcevasmed_r</t>
-  </si>
-  <si>
     <t>Passive parameter</t>
   </si>
   <si>
@@ -172,6 +106,12 @@
   </si>
   <si>
     <t>Second try</t>
+  </si>
+  <si>
+    <t>hip 45</t>
+  </si>
+  <si>
+    <t>hip 0</t>
   </si>
 </sst>
 </file>
@@ -207,13 +147,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,6 +1162,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hip 45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1269,7 +1226,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$25:$M$25</c:f>
+              <c:f>Sheet1!$C$28:$M$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1312,6 +1269,78 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACC6-4B96-BD35-7AC2FA5A0E77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hip 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-0.86116637052595346</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-40.76157509561375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.56080461803819748</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.81231279840241044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4150540537245337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.9185710207193232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.1814347850183431</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.78944240358681861</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.0188557366289526</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.1121215343371913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6FAA-4866-A911-A09CF3F11C0C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4250,7 +4279,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>291354</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>99593</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4278,16 +4307,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>78440</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>156883</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>392205</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>463364</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>42583</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>306481</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>121024</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4318,13 +4347,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>78440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>246530</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>185363</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4652,10 +4681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5385,11 +5414,11 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>44</v>
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C20">
         <v>0.317928889160771</v>
@@ -5426,8 +5455,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
       <c r="C21">
         <f>(C20-C$13)/C$13*100</f>
         <v>9.0874994561132502E-3</v>
@@ -5474,9 +5503,9 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C22">
         <v>0.70079674064287201</v>
@@ -5513,8 +5542,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
       <c r="C23">
         <f>(C22-0.7)/0.7*100</f>
         <v>0.11382009183886449</v>
@@ -5561,229 +5590,370 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24">
-        <v>0.27504427753983002</v>
-      </c>
-      <c r="D24">
-        <v>0.180864051255342</v>
-      </c>
-      <c r="E24">
-        <v>0.43239150102456497</v>
-      </c>
-      <c r="F24">
-        <v>0.45718836008415398</v>
-      </c>
-      <c r="G24">
-        <v>0.44980577152399098</v>
-      </c>
-      <c r="H24">
-        <v>0.300128911883002</v>
-      </c>
-      <c r="I24">
-        <v>0.19710041886212101</v>
-      </c>
-      <c r="K24">
-        <v>0.199265923653275</v>
-      </c>
-      <c r="L24">
-        <v>0.21556726988279401</v>
-      </c>
-      <c r="M24">
-        <v>0.19663902245023801</v>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
       <c r="C25">
-        <f>(C24-C$13)/C$13*100</f>
+        <v>0.44521300000000003</v>
+      </c>
+      <c r="D25">
+        <v>0.180864</v>
+      </c>
+      <c r="E25">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="F25">
+        <v>0.49440000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="H25">
+        <v>0.41689999999999999</v>
+      </c>
+      <c r="I25">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="J25">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="K25">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="L25">
+        <v>0.29267900000000002</v>
+      </c>
+      <c r="M25">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>0.31790000000000002</v>
+      </c>
+      <c r="D26">
+        <v>0.104</v>
+      </c>
+      <c r="E26">
+        <v>0.432</v>
+      </c>
+      <c r="F26">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="G26">
+        <v>0.42</v>
+      </c>
+      <c r="H26">
+        <v>0.33810000000000001</v>
+      </c>
+      <c r="I26">
+        <v>0.24540000000000001</v>
+      </c>
+      <c r="J26">
+        <v>0.25</v>
+      </c>
+      <c r="K26">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="L26">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="M26">
+        <v>0.19839999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>0.27504427753983002</v>
+      </c>
+      <c r="D27">
+        <v>0.180864051255342</v>
+      </c>
+      <c r="E27">
+        <v>0.43239150102456497</v>
+      </c>
+      <c r="F27">
+        <v>0.45718836008415398</v>
+      </c>
+      <c r="G27">
+        <v>0.44980577152399098</v>
+      </c>
+      <c r="H27">
+        <v>0.300128911883002</v>
+      </c>
+      <c r="I27">
+        <v>0.19710041886212101</v>
+      </c>
+      <c r="K27">
+        <v>0.199265923653275</v>
+      </c>
+      <c r="L27">
+        <v>0.21556726988279401</v>
+      </c>
+      <c r="M27">
+        <v>0.19663902245023801</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28">
+        <f>(C27-C$13)/C$13*100</f>
         <v>-13.480881554001256</v>
       </c>
-      <c r="D25">
-        <f t="shared" ref="D25:M25" si="8">(D24-D$13)/D$13*100</f>
+      <c r="D28">
+        <f t="shared" ref="D28:M28" si="8">(D27-D$13)/D$13*100</f>
         <v>73.907741591675006</v>
       </c>
-      <c r="E25">
+      <c r="E28">
         <f t="shared" si="8"/>
         <v>9.0625237167818867E-2</v>
       </c>
-      <c r="F25">
+      <c r="F28">
         <f t="shared" si="8"/>
         <v>4.1216648611369824E-2</v>
       </c>
-      <c r="G25">
+      <c r="G28">
         <f t="shared" si="8"/>
         <v>7.0966122676169041</v>
       </c>
-      <c r="H25">
+      <c r="H28">
         <f t="shared" si="8"/>
         <v>-11.230727038449572</v>
       </c>
-      <c r="I25">
+      <c r="I28">
         <f t="shared" si="8"/>
         <v>-19.68198090378117</v>
       </c>
-      <c r="J25">
+      <c r="J28">
         <f t="shared" si="8"/>
         <v>-100</v>
       </c>
-      <c r="K25">
+      <c r="K28">
         <f t="shared" si="8"/>
         <v>-0.56590636064121447</v>
       </c>
-      <c r="L25">
+      <c r="L28">
         <f t="shared" si="8"/>
         <v>-1.2518232328016416</v>
       </c>
-      <c r="M25">
+      <c r="M28">
         <f t="shared" si="8"/>
         <v>-0.88758949080745098</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.44521300000000003</v>
+      </c>
+      <c r="D29">
+        <v>0.180864</v>
+      </c>
+      <c r="E29">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="F29">
+        <v>0.49440000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="H29">
+        <v>0.41689999999999999</v>
+      </c>
+      <c r="I29">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="J29">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="K29">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="L29">
+        <v>0.29267900000000002</v>
+      </c>
+      <c r="M29">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>0.31790000000000002</v>
+      </c>
+      <c r="D30">
+        <v>0.104</v>
+      </c>
+      <c r="E30">
+        <v>0.432</v>
+      </c>
+      <c r="F30">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="G30">
+        <v>0.42</v>
+      </c>
+      <c r="H30">
+        <v>0.33810000000000001</v>
+      </c>
+      <c r="I30">
+        <v>0.24540000000000001</v>
+      </c>
+      <c r="J30">
+        <v>0.25</v>
+      </c>
+      <c r="K30">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="L30">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="M30">
+        <v>0.19839999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G44" t="s">
-        <v>26</v>
-      </c>
-      <c r="H44" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" t="s">
-        <v>28</v>
-      </c>
-      <c r="J44" t="s">
-        <v>29</v>
-      </c>
-      <c r="K44" t="s">
-        <v>30</v>
-      </c>
-      <c r="L44" t="s">
-        <v>31</v>
-      </c>
-      <c r="M44" t="s">
-        <v>32</v>
-      </c>
-      <c r="N44" t="s">
-        <v>33</v>
-      </c>
-      <c r="O44" t="s">
-        <v>34</v>
-      </c>
-      <c r="P44" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>36</v>
-      </c>
-      <c r="R44" t="s">
-        <v>37</v>
-      </c>
-      <c r="S44" t="s">
-        <v>38</v>
-      </c>
-      <c r="T44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V44" t="s">
-        <v>41</v>
-      </c>
-      <c r="W44" t="s">
-        <v>42</v>
+      <c r="C31">
+        <v>0.31516235210809801</v>
+      </c>
+      <c r="D31">
+        <v>6.1607961900561697E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.42957732405007498</v>
+      </c>
+      <c r="F31">
+        <v>0.453287730511301</v>
+      </c>
+      <c r="G31">
+        <v>0.43854322702564302</v>
+      </c>
+      <c r="H31">
+        <v>0.31132731137894798</v>
+      </c>
+      <c r="I31">
+        <v>0.23759275903756499</v>
+      </c>
+      <c r="K31">
+        <v>0.19881795742321201</v>
+      </c>
+      <c r="L31">
+        <v>0.21607583792693899</v>
+      </c>
+      <c r="M31">
+        <v>0.19619355087587501</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>0.317928889160771</v>
-      </c>
-      <c r="C45">
-        <v>0.70079674064287201</v>
-      </c>
-      <c r="D45">
-        <v>0.17060450569378599</v>
-      </c>
-      <c r="E45">
-        <v>0.70802054936171999</v>
-      </c>
-      <c r="F45">
-        <v>0.42704459805116801</v>
-      </c>
-      <c r="G45">
-        <v>0.69693452886853102</v>
-      </c>
-      <c r="H45">
-        <v>0.44820414428845101</v>
-      </c>
-      <c r="I45">
-        <v>0.69395337088414799</v>
-      </c>
-      <c r="J45">
-        <v>0.39747425206256698</v>
-      </c>
-      <c r="K45">
-        <v>0.79999999359030105</v>
-      </c>
-      <c r="L45">
-        <v>0.33835910801271601</v>
-      </c>
-      <c r="M45">
-        <v>0.69726547708197295</v>
-      </c>
-      <c r="N45">
-        <v>0.245525369483062</v>
-      </c>
-      <c r="O45">
-        <v>0.69993572020314598</v>
-      </c>
-      <c r="P45">
-        <v>0.24984576653162099</v>
-      </c>
-      <c r="Q45">
-        <v>0.70133491580469098</v>
-      </c>
-      <c r="R45">
-        <v>0.20014376388077901</v>
-      </c>
-      <c r="S45">
-        <v>0.69963467516214195</v>
-      </c>
-      <c r="T45">
-        <v>0.22289587902927099</v>
-      </c>
-      <c r="U45">
-        <v>0.56783493142832098</v>
-      </c>
-      <c r="V45">
-        <v>0.200618994686414</v>
-      </c>
-      <c r="W45">
-        <v>0.63613288686708103</v>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="C32">
+        <f>(C31-C$13)/C$13*100</f>
+        <v>-0.86116637052595346</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:I32" si="9">(D31-D$13)/D$13*100</f>
+        <v>-40.76157509561375</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="9"/>
+        <v>-0.56080461803819748</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="9"/>
+        <v>-0.81231279840241044</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>4.4150540537245337</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="9"/>
+        <v>-7.9185710207193232</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="9"/>
+        <v>-3.1814347850183431</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32" si="10">(J31-J$13)/J$13*100</f>
+        <v>-100</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32" si="11">(K31-K$13)/K$13*100</f>
+        <v>-0.78944240358681861</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ref="L32" si="12">(L31-L$13)/L$13*100</f>
+        <v>-1.0188557366289526</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ref="M32" si="13">(M31-M$13)/M$13*100</f>
+        <v>-1.1121215343371913</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Result of batch processing (Hip 0, 45, 90)
For one parameter and all muscles except tfl, sart.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4881C686-4808-463C-8CA3-753A4EEED6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89958664-FFF6-4D5B-B602-6B4E743377B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>bflh_r</t>
   </si>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -156,10 +156,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,11 +1121,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tendon Slack lenght_Hip45</a:t>
+              <a:t>Tendon Slack lenght</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32600290371913082"/>
+          <c:y val="3.5087719298245612E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1942,6 +1953,7 @@
         <c:axId val="420352799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2018,6 +2030,622 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tendon Slack lenght</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$36:$L$36</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$37:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-2.2551074558826101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7532495083177701E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.479702685562298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.850527627978648</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4601551207317999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.89133051648954298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.93365135722887804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7494729415423103E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.167889566618353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.116238772075476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C53C-4FFC-AE0B-3080960638FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$36:$L$36</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.17425431557024901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16881336560996599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.96516941532540701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.67035812182452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.24723281489919899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.8117478771300504E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.29199441559712302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.7916480588952001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.154440868332335</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.95430749496676E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C53C-4FFC-AE0B-3080960638FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$39:$L$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.0404267397660399E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.63312766126432896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.73233585658855704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.0237988787135199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.3490168539606202</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7015500217260503E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.02782760210235E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.191829499314213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.361570688514122</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.24166257818223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C53C-4FFC-AE0B-3080960638FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="984742879"/>
+        <c:axId val="984746623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="984742879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984746623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="984746623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984742879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2237,6 +2865,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4199,6 +4867,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4376,6 +5547,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>179295</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>67233</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>246530</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B34432-2C81-44B0-89AA-752335A7BC2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4681,15 +5890,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5414,10 +6624,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C20">
@@ -5455,8 +6665,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
       <c r="C21">
         <f>(C20-C$13)/C$13*100</f>
         <v>9.0874994561132502E-3</v>
@@ -5503,8 +6713,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C22">
@@ -5542,8 +6752,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23">
         <f>(C22-0.7)/0.7*100</f>
         <v>0.11382009183886449</v>
@@ -5706,7 +6916,7 @@
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C27">
@@ -5742,7 +6952,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="5"/>
       <c r="C28">
         <f>(C27-C$13)/C$13*100</f>
         <v>-13.480881554001256</v>
@@ -5946,8 +7156,166 @@
         <v>-1.1121215343371913</v>
       </c>
     </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>-2.2551074558826101</v>
+      </c>
+      <c r="D37">
+        <v>9.7532495083177701E-3</v>
+      </c>
+      <c r="E37">
+        <v>-0.479702685562298</v>
+      </c>
+      <c r="F37">
+        <v>-0.850527627978648</v>
+      </c>
+      <c r="G37">
+        <v>2.4601551207317999E-2</v>
+      </c>
+      <c r="H37">
+        <v>-0.89133051648954298</v>
+      </c>
+      <c r="I37">
+        <v>-0.93365135722887804</v>
+      </c>
+      <c r="J37">
+        <v>3.7494729415423103E-2</v>
+      </c>
+      <c r="K37">
+        <v>0.167889566618353</v>
+      </c>
+      <c r="L37">
+        <v>0.116238772075476</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>-0.17425431557024901</v>
+      </c>
+      <c r="D38">
+        <v>0.16881336560996599</v>
+      </c>
+      <c r="E38">
+        <v>-0.96516941532540701</v>
+      </c>
+      <c r="F38">
+        <v>-1.67035812182452</v>
+      </c>
+      <c r="G38">
+        <v>-0.24723281489919899</v>
+      </c>
+      <c r="H38">
+        <v>-9.8117478771300504E-2</v>
+      </c>
+      <c r="I38">
+        <v>-0.29199441559712302</v>
+      </c>
+      <c r="J38">
+        <v>-3.7916480588952001E-2</v>
+      </c>
+      <c r="K38">
+        <v>-0.154440868332335</v>
+      </c>
+      <c r="L38">
+        <v>-7.95430749496676E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3">
+        <v>90</v>
+      </c>
+      <c r="C39">
+        <v>8.0404267397660399E-3</v>
+      </c>
+      <c r="D39">
+        <v>-0.63312766126432896</v>
+      </c>
+      <c r="E39">
+        <v>-0.73233585658855704</v>
+      </c>
+      <c r="F39">
+        <v>-1.0237988787135199</v>
+      </c>
+      <c r="G39">
+        <v>-2.3490168539606202</v>
+      </c>
+      <c r="H39">
+        <v>4.7015500217260503E-3</v>
+      </c>
+      <c r="I39">
+        <v>1.02782760210235E-2</v>
+      </c>
+      <c r="J39">
+        <v>-0.191829499314213</v>
+      </c>
+      <c r="K39">
+        <v>-0.361570688514122</v>
+      </c>
+      <c r="L39">
+        <v>-0.24166257818223</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A35:N35"/>
+    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B20:B21"/>

</xml_diff>

<commit_message>
Result of simulation for 2 unknown parameter Hip 90, 0
Simulation did not converge on Hip45 deg
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyCloud\GitHub\Muscle_Tendon_Passive_Parameter_Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89958664-FFF6-4D5B-B602-6B4E743377B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D1C38C-5BDB-4333-BC5F-80E6B366D6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F14FCE5F-3BE0-4D3F-B97B-F4447167A072}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$R$9</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$A$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$B$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$C$6:$L$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$R$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>bflh_r</t>
   </si>
@@ -112,6 +120,18 @@
   </si>
   <si>
     <t>hip 0</t>
+  </si>
+  <si>
+    <t>Hip90</t>
+  </si>
+  <si>
+    <t>Hip0</t>
+  </si>
+  <si>
+    <t>Tendon</t>
+  </si>
+  <si>
+    <t>Passive</t>
   </si>
 </sst>
 </file>
@@ -2705,6 +2725,1074 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Hip90</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tendon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.20933301631738563</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.5628048136439046</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.17939983802431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.5802296074691264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.6388097611398094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.206171132883226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39683241308956835</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.99586333088756118</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.1129521822290303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.77222101071311389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67B7-4AE6-A842-377C85204596}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Passive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.0774279390737116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.447472610850726</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.494754569119143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8274333111987273</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.6892465335384195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.4102310239672806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.0265467069712844</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.757588043798572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5462721830521486</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.085787371171727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67B7-4AE6-A842-377C85204596}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="420355295"/>
+        <c:axId val="420352799"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="420355295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420352799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420352799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420355295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Hip0</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tendon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$13:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-6.0638805245024967</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.1812276639749009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.75563453065732367</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.1285361607190101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60949576985661713</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.1083509631116906</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0048814458152897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.42809964725908584</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.509618458293877</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.2273105196630527</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25BE-40E5-B997-0547B23C9044}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Passive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$14:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10.938533254947441</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2519519202434326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.109304132319288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.647692811284433</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.200997357598431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.609304147681863</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2127851929891502</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7279523327348656</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.22214837439958</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7345858670492902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-25BE-40E5-B997-0547B23C9044}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="420355295"/>
+        <c:axId val="420352799"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="420355295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420352799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="420352799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="420355295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2905,6 +3993,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5370,6 +6538,994 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5554,16 +7710,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>179295</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>67233</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>963707</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>33616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>246530</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>134470</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>829236</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5585,6 +7741,87 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>372036</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>125973</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0622945C-9E67-464A-A247-88FF9D9D4CBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>352986</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>49773</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F4C446-66C7-4D11-89E3-A0E7D7289642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5892,8 +8129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B64B4-881C-490D-8F4B-C299AF3F405C}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7327,4 +9564,502 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C48658-27FD-49CA-97E1-F6947C850BC8}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.31797313845694503</v>
+      </c>
+      <c r="D2">
+        <v>0.104999391749968</v>
+      </c>
+      <c r="E2">
+        <v>0.43293364469715501</v>
+      </c>
+      <c r="F2">
+        <v>0.45724542642978899</v>
+      </c>
+      <c r="G2">
+        <v>0.41325493206287101</v>
+      </c>
+      <c r="H2">
+        <v>0.33813888376453399</v>
+      </c>
+      <c r="I2">
+        <v>0.245475137444266</v>
+      </c>
+      <c r="J2">
+        <v>0.20046131582902799</v>
+      </c>
+      <c r="K2">
+        <v>0.218329273203307</v>
+      </c>
+      <c r="L2">
+        <v>0.19846393006047999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="C3">
+        <v>0.7</v>
+      </c>
+      <c r="D3">
+        <v>0.7</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
+        <v>0.7</v>
+      </c>
+      <c r="G3">
+        <v>0.7</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
+      </c>
+      <c r="J3">
+        <v>0.7</v>
+      </c>
+      <c r="K3">
+        <v>0.7</v>
+      </c>
+      <c r="L3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0.31863876121875601</v>
+      </c>
+      <c r="D4">
+        <v>0.102308462283903</v>
+      </c>
+      <c r="E4">
+        <v>0.42782762599284402</v>
+      </c>
+      <c r="F4">
+        <v>0.450019898822547</v>
+      </c>
+      <c r="G4">
+        <v>0.40648246989783299</v>
+      </c>
+      <c r="H4">
+        <v>0.33883602853191003</v>
+      </c>
+      <c r="I4">
+        <v>0.24644926235572101</v>
+      </c>
+      <c r="J4">
+        <v>0.19846499509207199</v>
+      </c>
+      <c r="K4">
+        <v>0.21589937279274601</v>
+      </c>
+      <c r="L4">
+        <v>0.19693134989386599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>0.69245800442648398</v>
+      </c>
+      <c r="D5">
+        <v>0.78013230827595503</v>
+      </c>
+      <c r="E5">
+        <v>0.77346328198383396</v>
+      </c>
+      <c r="F5">
+        <v>0.74079203317839104</v>
+      </c>
+      <c r="G5">
+        <v>0.63217527426523101</v>
+      </c>
+      <c r="H5">
+        <v>0.69012838283222899</v>
+      </c>
+      <c r="I5">
+        <v>0.69281417305120097</v>
+      </c>
+      <c r="J5">
+        <v>0.74030311630658996</v>
+      </c>
+      <c r="K5">
+        <v>0.73882390528136499</v>
+      </c>
+      <c r="L5">
+        <v>0.72160051159820204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>(C4-C2)/C2*100</f>
+        <v>0.20933301631738563</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:L7" si="0">(D4-D2)/D2*100</f>
+        <v>-2.5628048136439046</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-1.17939983802431</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-1.5802296074691264</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-1.6388097611398094</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.206171132883226</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.39683241308956835</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-0.99586333088756118</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-1.1129521822290303</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>-0.77222101071311389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>(C5-C3)/C3*100</f>
+        <v>-1.0774279390737116</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>11.447472610850726</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10.494754569119143</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>5.8274333111987273</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>-9.6892465335384195</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-1.4102310239672806</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>-1.0265467069712844</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>5.757588043798572</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>5.5462721830521486</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>3.085787371171727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.31797313845694503</v>
+      </c>
+      <c r="D9">
+        <v>0.104999391749968</v>
+      </c>
+      <c r="E9">
+        <v>0.43293364469715501</v>
+      </c>
+      <c r="F9">
+        <v>0.45724542642978899</v>
+      </c>
+      <c r="G9">
+        <v>0.43919738099670702</v>
+      </c>
+      <c r="H9">
+        <v>0.32187501872910301</v>
+      </c>
+      <c r="I9">
+        <v>0.245475137444266</v>
+      </c>
+      <c r="J9">
+        <v>0.20046131582902799</v>
+      </c>
+      <c r="K9">
+        <v>0.218329273203307</v>
+      </c>
+      <c r="L9">
+        <v>0.19846393006047999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.7</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="E10">
+        <v>0.7</v>
+      </c>
+      <c r="F10">
+        <v>0.7</v>
+      </c>
+      <c r="G10">
+        <v>0.7</v>
+      </c>
+      <c r="H10">
+        <v>0.7</v>
+      </c>
+      <c r="I10">
+        <v>0.7</v>
+      </c>
+      <c r="J10">
+        <v>0.7</v>
+      </c>
+      <c r="K10">
+        <v>0.7</v>
+      </c>
+      <c r="L10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>0.29869162724090498</v>
+      </c>
+      <c r="D11">
+        <v>0.103759109887612</v>
+      </c>
+      <c r="E11">
+        <v>0.42966224858299001</v>
+      </c>
+      <c r="F11">
+        <v>0.45208524644929499</v>
+      </c>
+      <c r="G11">
+        <v>0.441874270455203</v>
+      </c>
+      <c r="H11">
+        <v>0.311870013484421</v>
+      </c>
+      <c r="I11">
+        <v>0.23564414921067101</v>
+      </c>
+      <c r="J11">
+        <v>0.199603141643073</v>
+      </c>
+      <c r="K11">
+        <v>0.21503333419517101</v>
+      </c>
+      <c r="L11">
+        <v>0.196028161369111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>0.77656973278463204</v>
+      </c>
+      <c r="D12">
+        <v>0.75076366344170398</v>
+      </c>
+      <c r="E12">
+        <v>0.79176512892623496</v>
+      </c>
+      <c r="F12">
+        <v>0.78853384967899098</v>
+      </c>
+      <c r="G12">
+        <v>0.64959301849681095</v>
+      </c>
+      <c r="H12">
+        <v>0.78826512903377299</v>
+      </c>
+      <c r="I12">
+        <v>0.757489496350924</v>
+      </c>
+      <c r="J12">
+        <v>0.71909566632914401</v>
+      </c>
+      <c r="K12">
+        <v>0.78555503862079701</v>
+      </c>
+      <c r="L12">
+        <v>0.76114210106934499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>(C11-C9)/C9*100</f>
+        <v>-6.0638805245024967</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:L13" si="1">(D11-D9)/D9*100</f>
+        <v>-1.1812276639749009</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-0.75563453065732367</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>-1.1285361607190101</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.60949576985661713</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>-3.1083509631116906</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>-4.0048814458152897</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>-0.42809964725908584</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-1.509618458293877</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>-1.2273105196630527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>(C12-C10)/C10*100</f>
+        <v>10.938533254947441</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:L14" si="2">(D12-D10)/D10*100</f>
+        <v>7.2519519202434326</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>13.109304132319288</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>12.647692811284433</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>-7.200997357598431</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>12.609304147681863</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>8.2127851929891502</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>2.7279523327348656</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>12.22214837439958</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>8.7345858670492902</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>